<commit_message>
made some more changes to debugger
</commit_message>
<xml_diff>
--- a/projects/02/ALU Debugger.xlsx
+++ b/projects/02/ALU Debugger.xlsx
@@ -47,9 +47,6 @@
     <t>ny</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>1/0</t>
+  </si>
+  <si>
+    <t>f (1 for add)</t>
   </si>
 </sst>
 </file>
@@ -555,20 +555,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="5.46484375" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" customWidth="1"/>
+    <col min="2" max="2" width="10.06640625" customWidth="1"/>
     <col min="3" max="34" width="2.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B2" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -609,56 +610,56 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="5">
         <v>1</v>
@@ -713,70 +714,72 @@
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
       <c r="C4" s="8">
         <f>IF($B$4=1,0,C$3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:R4" si="0">IF($B$4=1,0,D$3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="8">
         <f>S3</f>
@@ -852,67 +855,67 @@
       </c>
       <c r="C5" s="8">
         <f>IF($B$5=1,IF(C4=1,0,1),C4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" ref="D5:R5" si="2">IF($B$5=1,IF(D4=1,0,1),D4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="8">
         <f>S4</f>
@@ -983,204 +986,208 @@
       <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
       <c r="C6" s="8">
         <f>C5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ref="D6:R7" si="3">D5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="8">
         <f>IF($B$6=1,0,S5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="9">
         <f t="shared" ref="T6:AH6" si="4">IF($B$6=1,0,T5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
       <c r="C7" s="11">
         <f>C6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="11">
         <f>IF($B$7=1,IF(S6=1,0,1),S6)</f>
@@ -1249,74 +1256,74 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="14">
-        <f>IF($B$8=1,C7+S7,0)</f>
-        <v>1</v>
+        <f>IF($B$8=1,IF(C7+S7=2,0,C7+S7),IF(C7+S7=2,1,0))</f>
+        <v>0</v>
       </c>
       <c r="D8" s="15">
-        <f t="shared" ref="D8:R8" si="6">IF($B$8=1,D7+T7,0)</f>
-        <v>1</v>
+        <f t="shared" ref="D8:R8" si="6">IF($B$8=1,IF(D7+T7=2,0,D7+T7),IF(D7+T7=2,1,0))</f>
+        <v>0</v>
       </c>
       <c r="E8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
@@ -1337,25 +1344,75 @@
     </row>
     <row r="9" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="17">
+        <f>IF($B$9=1,IF(C8=1,0,1),C8)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
+        <f t="shared" ref="D9:R9" si="7">IF($B$9=1,IF(D8=1,0,1),D8)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q9" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R9" s="19">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -1380,67 +1437,67 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4">
         <f>C9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ref="D10:R10" si="7">D9</f>
-        <v>0</v>
+        <f t="shared" ref="D10:R10" si="8">D9</f>
+        <v>1</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>

</xml_diff>

<commit_message>
more changes to debugger
</commit_message>
<xml_diff>
--- a/projects/02/ALU Debugger.xlsx
+++ b/projects/02/ALU Debugger.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
   <si>
     <t>x input</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>ALU-DeBu</t>
+  </si>
+  <si>
+    <t>Carry</t>
   </si>
 </sst>
 </file>
@@ -315,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -403,6 +406,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AI15"/>
+  <dimension ref="B2:AI16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -714,7 +726,7 @@
     </row>
     <row r="4" spans="2:35" ht="15" thickBot="1">
       <c r="B4" s="14" t="str">
-        <f>IF(C15=0,"PASS","FAIL")</f>
+        <f>IF(C16=0,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
@@ -1528,76 +1540,73 @@
       <c r="AH11" s="22"/>
       <c r="AI11" s="22"/>
     </row>
-    <row r="12" spans="2:35" ht="15.75" thickBot="1">
+    <row r="12" spans="2:35" ht="15">
       <c r="B12" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="22">
-        <f>VLOOKUP(testNo,testResults,41,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="35">
-        <f>IF($C$12=1,IF(D11=1,0,1),D11)</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="36">
-        <f t="shared" ref="E12:S12" si="7">IF($C$12=1,IF(E11=1,0,1),E11)</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="M12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="36">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="S12" s="37">
-        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="39">
+        <f t="shared" ref="D12:R12" si="7">IF(T10+D10+E11&gt;1,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S12" s="41">
+        <f>IF(AI10+S10+T11&gt;1,1,0)</f>
         <v>1</v>
       </c>
       <c r="T12" s="22"/>
@@ -1617,74 +1626,74 @@
       <c r="AH12" s="22"/>
       <c r="AI12" s="22"/>
     </row>
-    <row r="13" spans="2:35" ht="15">
+    <row r="13" spans="2:35" ht="15.75" thickBot="1">
       <c r="B13" s="21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="38">
-        <f>D12</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="38">
-        <f t="shared" ref="E13:S13" si="8">E12</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="M13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="P13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="R13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="S13" s="38">
-        <f t="shared" si="8"/>
-        <v>1</v>
+      <c r="D13" s="35">
+        <f>IF($C$13=1,IF(D11=1,0,1),D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="36">
+        <f t="shared" ref="E13:S13" si="8">IF($C$13=1,IF(E11=1,0,1),E11)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="T13" s="22"/>
       <c r="U13" s="22"/>
@@ -1705,72 +1714,72 @@
     </row>
     <row r="14" spans="2:35" ht="15">
       <c r="B14" s="21" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(D14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(E14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(F14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(G14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(H14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(I14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(J14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(K14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(L14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(M14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(N14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(O14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(P14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Q14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(R14)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(S14)+39,FALSE))</f>
-        <v>1</v>
+      <c r="D14" s="38">
+        <f>D13</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="38">
+        <f t="shared" ref="E14:S14" si="9">E13</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="T14" s="22"/>
       <c r="U14" s="22"/>
@@ -1791,75 +1800,72 @@
     </row>
     <row r="15" spans="2:35" ht="15">
       <c r="B15" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="22">
-        <f>COUNTIF(D15:S15,"x")</f>
-        <v>15</v>
-      </c>
-      <c r="D15" s="22" t="str">
-        <f>IF(D13&lt;&gt;D14,"x","")</f>
-        <v>x</v>
-      </c>
-      <c r="E15" s="22" t="str">
-        <f>IF(E13&lt;&gt;E14,"x","")</f>
-        <v>x</v>
-      </c>
-      <c r="F15" s="22" t="str">
-        <f t="shared" ref="E15:S15" si="9">IF(F13&lt;&gt;F14,"x","")</f>
-        <v>x</v>
-      </c>
-      <c r="G15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="H15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="I15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="J15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="K15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="L15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="M15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="N15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="O15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="P15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="Q15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="R15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v>x</v>
-      </c>
-      <c r="S15" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <v>37</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(D15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(E15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(F15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(G15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(H15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(I15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(J15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(K15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(L15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(M15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(N15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(O15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(P15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Q15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(R15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(S15)+39,FALSE))</f>
+        <v>1</v>
       </c>
       <c r="T15" s="22"/>
       <c r="U15" s="22"/>
@@ -1877,6 +1883,95 @@
       <c r="AG15" s="22"/>
       <c r="AH15" s="22"/>
       <c r="AI15" s="22"/>
+    </row>
+    <row r="16" spans="2:35" ht="15">
+      <c r="B16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="22">
+        <f>COUNTIF(D16:S16,"x")</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="22" t="str">
+        <f>IF(D14&lt;&gt;D15,"x","")</f>
+        <v/>
+      </c>
+      <c r="E16" s="22" t="str">
+        <f>IF(E14&lt;&gt;E15,"x","")</f>
+        <v/>
+      </c>
+      <c r="F16" s="22" t="str">
+        <f t="shared" ref="E16:S16" si="10">IF(F14&lt;&gt;F15,"x","")</f>
+        <v/>
+      </c>
+      <c r="G16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="I16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="K16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="L16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="O16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="P16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="R16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="S16" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>x</v>
+      </c>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AI16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1905,7 +2000,7 @@
   <dimension ref="B1:BH38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
built the ALU fully in excel
</commit_message>
<xml_diff>
--- a/projects/02/ALU Debugger.xlsx
+++ b/projects/02/ALU Debugger.xlsx
@@ -162,7 +162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +197,16 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="monti"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="monti"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="monti"/>
     </font>
   </fonts>
@@ -318,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -345,15 +355,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,13 +409,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,7 +702,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,7 +713,7 @@
   <dimension ref="B2:AI16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -721,1257 +734,1243 @@
     </row>
     <row r="3" spans="2:35">
       <c r="B3" s="16">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:35" ht="15" thickBot="1">
       <c r="B4" s="14" t="str">
         <f>IF(C16=0,"PASS","FAIL")</f>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="2:35">
       <c r="C5" s="17"/>
-      <c r="D5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="20"/>
+      <c r="D5" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
+      <c r="AI5" s="38"/>
     </row>
     <row r="6" spans="2:35" ht="15">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(D6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(E6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(F6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(G6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(H6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(I6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(J6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(K6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(L6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(M6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(N6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(O6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(P6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Q6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(R6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="25">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(S6)-2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="23">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(T6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="U6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(U6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="V6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(V6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="W6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(W6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="X6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(X6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="Y6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Y6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="Z6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Z6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AA6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AA6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AB6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AB6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AC6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AC6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AD6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AD6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AE6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AE6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AF6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AF6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AG6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AG6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AH6" s="24">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AH6)+1,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AI6" s="25">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AI6)+1,FALSE))</f>
-        <v>1</v>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(D6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(E6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(F6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(G6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(H6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(I6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(J6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(K6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(L6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(M6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(N6)-1,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(O6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(P6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Q6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(R6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(S6)-1,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="20">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(T6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(U6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(V6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(W6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(X6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Y6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Z6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AA6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AB6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AC6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AC6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AD6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AE6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AF6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AF6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AG6),FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="21">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AH6),FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AI6" s="22">
+        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(AI6),FALSE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:35" ht="15">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <f>VLOOKUP(testNo,testResults,36,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
         <f>IF($C$7=1,0,D$6)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="24">
         <f t="shared" ref="E7:S7" si="0">IF($C$7=1,0,E$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="26">
+        <v>1</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="23">
         <f>T6</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="27">
+        <v>0</v>
+      </c>
+      <c r="U7" s="24">
         <f t="shared" ref="U7:AI8" si="1">U6</f>
-        <v>1</v>
-      </c>
-      <c r="V7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="W7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="X7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AA7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AB7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AC7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AD7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AE7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AF7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AG7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AH7" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AI7" s="28">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="V7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Y7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Z7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AI7" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:35" ht="15">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="19">
         <f>VLOOKUP(testNo,testResults,37,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="23">
         <f>IF($C$8=1,IF(D7=1,0,1),D7)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="24">
         <f t="shared" ref="E8:S8" si="2">IF($C$8=1,IF(E7=1,0,1),E7)</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="S8" s="28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="T8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S8" s="25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T8" s="23">
         <f>T7</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="V8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="W8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="X8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AA8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AB8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AC8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AD8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AE8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AF8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AG8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AH8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AI8" s="28">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Y8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Z8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AI8" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:35" ht="15">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="19">
         <f>VLOOKUP(testNo,testResults,38,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="23">
         <f>D8</f>
         <v>1</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="24">
         <f t="shared" ref="E9:S10" si="3">E8</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="27">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I9" s="27">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K9" s="27">
+        <v>0</v>
+      </c>
+      <c r="K9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L9" s="27">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M9" s="27">
+        <v>0</v>
+      </c>
+      <c r="M9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O9" s="27">
+        <v>0</v>
+      </c>
+      <c r="O9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P9" s="27">
+      <c r="P9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="27">
+      <c r="Q9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R9" s="27">
+      <c r="R9" s="24">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9" s="25">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T9" s="26">
+      <c r="T9" s="23">
         <f>IF($C$9=1,0,T8)</f>
         <v>0</v>
       </c>
-      <c r="U9" s="27">
+      <c r="U9" s="24">
         <f t="shared" ref="U9:AI9" si="4">IF($C$9=1,0,U8)</f>
         <v>0</v>
       </c>
-      <c r="V9" s="27">
+      <c r="V9" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W9" s="27">
+      <c r="W9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X9" s="27">
+        <v>1</v>
+      </c>
+      <c r="X9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="27">
+      <c r="AB9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC9" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="27">
+      <c r="AE9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="27">
+      <c r="AG9" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH9" s="27">
+      <c r="AH9" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AI9" s="28">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:35" ht="15.75" thickBot="1">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="19">
         <f>VLOOKUP(testNo,testResults,39,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="26">
         <f>D9</f>
         <v>1</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H10" s="30">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I10" s="30">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="30">
+        <v>0</v>
+      </c>
+      <c r="K10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L10" s="30">
+        <v>0</v>
+      </c>
+      <c r="L10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M10" s="30">
+        <v>0</v>
+      </c>
+      <c r="M10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O10" s="30">
+        <v>0</v>
+      </c>
+      <c r="O10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P10" s="30">
+      <c r="P10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R10" s="30">
+      <c r="R10" s="27">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="S10" s="31">
+      <c r="S10" s="28">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T10" s="29">
+      <c r="T10" s="26">
         <f>IF($C$10=1,IF(T9=1,0,1),T9)</f>
         <v>1</v>
       </c>
-      <c r="U10" s="30">
+      <c r="U10" s="27">
         <f t="shared" ref="U10:AI10" si="5">IF($C$10=1,IF(U9=1,0,1),U9)</f>
         <v>1</v>
       </c>
-      <c r="V10" s="30">
+      <c r="V10" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W10" s="30">
+      <c r="W10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="X10" s="30">
+        <v>0</v>
+      </c>
+      <c r="X10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Y10" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Z10" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AA10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AB10" s="30">
+      <c r="AB10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AC10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AD10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AE10" s="30">
+      <c r="AE10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AF10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AG10" s="30">
+      <c r="AG10" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AH10" s="30">
+      <c r="AH10" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AI10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:35" ht="15">
-      <c r="B11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="22">
-        <f>VLOOKUP(testNo,testResults,40,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="32">
-        <f>IF($C$11=1,IF(D10+T10=2,0,D10+T10),IF(D10+T10=2,1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="33">
-        <f t="shared" ref="E11:S11" si="6">IF($C$11=1,IF(E10+U10=2,0,E10+U10),IF(E10+U10=2,1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="33">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S11" s="34">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="22"/>
-      <c r="AI11" s="22"/>
+    <row r="11" spans="2:35" s="39" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="40">
+        <f t="shared" ref="D11:Q11" si="6">IF(T10+D10+E11&gt;1,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R11" s="41">
+        <f>IF(AH10+R10+S11&gt;1,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S11" s="42">
+        <f>IF(AI10+S10+T12&gt;1,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="2:35" ht="15">
-      <c r="B12" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="39">
-        <f t="shared" ref="D12:R12" si="7">IF(T10+D10+E11&gt;1,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="F12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="M12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="40">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="S12" s="41">
-        <f>IF(AI10+S10+T11&gt;1,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="22"/>
-      <c r="AD12" s="22"/>
-      <c r="AE12" s="22"/>
-      <c r="AF12" s="22"/>
-      <c r="AG12" s="22"/>
-      <c r="AH12" s="22"/>
-      <c r="AI12" s="22"/>
+      <c r="B12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19">
+        <f>VLOOKUP(testNo,testResults,40,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <f t="shared" ref="D12:R12" si="7">IF($C$12&lt;&gt;1,IF(AND(D10=1,T10=1),1,0),IF(MOD(T10+D10+E11,2)=0,0,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="31">
+        <f>IF($C$12&lt;&gt;1,IF(AND(S10=1,AI10=1),1,0),IF(MOD(AI10+S10+T11,2)=0,0,1))</f>
+        <v>1</v>
+      </c>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="19"/>
+      <c r="AI12" s="19"/>
     </row>
     <row r="13" spans="2:35" ht="15.75" thickBot="1">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="35">
-        <f>IF($C$13=1,IF(D11=1,0,1),D11)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="36">
-        <f t="shared" ref="E13:S13" si="8">IF($C$13=1,IF(E11=1,0,1),E11)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="22"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="22"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="22"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="22"/>
-      <c r="AI13" s="22"/>
+      <c r="C13" s="19">
+        <f>VLOOKUP(testNo,testResults,41,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="32">
+        <f>IF($C$13=1,IF(D12=1,0,1),D12)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <f>IF($C$13=1,IF(E12=1,0,1),E12)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="33">
+        <f>IF($C$13=1,IF(F12=1,0,1),F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <f>IF($C$13=1,IF(G12=1,0,1),G12)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="33">
+        <f>IF($C$13=1,IF(H12=1,0,1),H12)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="33">
+        <f>IF($C$13=1,IF(I12=1,0,1),I12)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="33">
+        <f>IF($C$13=1,IF(J12=1,0,1),J12)</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="33">
+        <f>IF($C$13=1,IF(K12=1,0,1),K12)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="33">
+        <f>IF($C$13=1,IF(L12=1,0,1),L12)</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="33">
+        <f>IF($C$13=1,IF(M12=1,0,1),M12)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="33">
+        <f>IF($C$13=1,IF(N12=1,0,1),N12)</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="33">
+        <f>IF($C$13=1,IF(O12=1,0,1),O12)</f>
+        <v>1</v>
+      </c>
+      <c r="P13" s="33">
+        <f>IF($C$13=1,IF(P12=1,0,1),P12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="33">
+        <f>IF($C$13=1,IF(Q12=1,0,1),Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="33">
+        <f>IF($C$13=1,IF(R12=1,0,1),R12)</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="34">
+        <f>IF($C$13=1,IF(S12=1,0,1),S12)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AH13" s="19"/>
+      <c r="AI13" s="19"/>
     </row>
     <row r="14" spans="2:35" ht="15">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="38">
+      <c r="C14" s="19"/>
+      <c r="D14" s="35">
         <f>D13</f>
         <v>0</v>
       </c>
-      <c r="E14" s="38">
-        <f t="shared" ref="E14:S14" si="9">E13</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S14" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="22"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="22"/>
-      <c r="AG14" s="22"/>
-      <c r="AH14" s="22"/>
-      <c r="AI14" s="22"/>
+      <c r="E14" s="35">
+        <f t="shared" ref="E14:S14" si="8">E13</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S14" s="35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
+      <c r="AI14" s="19"/>
     </row>
     <row r="15" spans="2:35" ht="15">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(D15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(E15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(F15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(G15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(H15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(I15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(J15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(K15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(L15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(M15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(N15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(O15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(P15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(Q15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(R15)+39,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="22">
-        <f>VALUE(VLOOKUP(testNo,testResults,COLUMN(S15)+39,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="22"/>
-      <c r="AB15" s="22"/>
-      <c r="AC15" s="22"/>
-      <c r="AD15" s="22"/>
-      <c r="AE15" s="22"/>
-      <c r="AF15" s="22"/>
-      <c r="AG15" s="22"/>
-      <c r="AH15" s="22"/>
-      <c r="AI15" s="22"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19">
+        <f t="shared" ref="D15:S15" si="9">VALUE(VLOOKUP(testNo,testResults,COLUMN(D15)+39,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="S15" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
     </row>
     <row r="16" spans="2:35" ht="15">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="19">
         <f>COUNTIF(D16:S16,"x")</f>
-        <v>1</v>
-      </c>
-      <c r="D16" s="22" t="str">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19" t="str">
         <f>IF(D14&lt;&gt;D15,"x","")</f>
         <v/>
       </c>
-      <c r="E16" s="22" t="str">
+      <c r="E16" s="19" t="str">
         <f>IF(E14&lt;&gt;E15,"x","")</f>
         <v/>
       </c>
-      <c r="F16" s="22" t="str">
-        <f t="shared" ref="E16:S16" si="10">IF(F14&lt;&gt;F15,"x","")</f>
+      <c r="F16" s="19" t="str">
+        <f t="shared" ref="F16:S16" si="10">IF(F14&lt;&gt;F15,"x","")</f>
         <v/>
       </c>
-      <c r="G16" s="22" t="str">
+      <c r="G16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="H16" s="22" t="str">
+      <c r="H16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I16" s="22" t="str">
+      <c r="I16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="J16" s="22" t="str">
+      <c r="J16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="K16" s="22" t="str">
+      <c r="K16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="L16" s="22" t="str">
+      <c r="L16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="M16" s="22" t="str">
+      <c r="M16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="N16" s="22" t="str">
+      <c r="N16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="O16" s="22" t="str">
+      <c r="O16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="P16" s="22" t="str">
+      <c r="P16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="Q16" s="22" t="str">
+      <c r="Q16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="R16" s="22" t="str">
+      <c r="R16" s="19" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="S16" s="22" t="str">
+      <c r="S16" s="19" t="str">
         <f t="shared" si="10"/>
-        <v>x</v>
-      </c>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-      <c r="AC16" s="22"/>
-      <c r="AD16" s="22"/>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AI16" s="22"/>
+        <v/>
+      </c>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="19"/>
+      <c r="AF16" s="19"/>
+      <c r="AG16" s="19"/>
+      <c r="AH16" s="19"/>
+      <c r="AI16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2000,7 +1999,7 @@
   <dimension ref="B1:BH38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C20" sqref="C20:BH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9719,7 +9718,7 @@
         <v>19</v>
       </c>
       <c r="E36" s="5" t="str">
-        <f t="shared" ref="E36:T38" si="12">MID($D36,COLUMN(E36)-3,1)</f>
+        <f t="shared" ref="E36:S38" si="12">MID($D36,COLUMN(E36)-3,1)</f>
         <v>0</v>
       </c>
       <c r="F36" s="5" t="str">
@@ -9786,7 +9785,7 @@
         <v>20</v>
       </c>
       <c r="V36" s="5" t="str">
-        <f t="shared" ref="V36:AK38" si="13">MID($U36,COLUMN(V36)-20,1)</f>
+        <f t="shared" ref="V36:AJ38" si="13">MID($U36,COLUMN(V36)-20,1)</f>
         <v>0</v>
       </c>
       <c r="W36" s="5" t="str">
@@ -9871,7 +9870,7 @@
         <v>31</v>
       </c>
       <c r="AS36" s="5" t="str">
-        <f t="shared" ref="AS36:BH38" si="14">MID($AR36,COLUMN(AS36)-43,1)</f>
+        <f t="shared" ref="AS36:BG38" si="14">MID($AR36,COLUMN(AS36)-43,1)</f>
         <v>1</v>
       </c>
       <c r="AT36" s="5" t="str">

</xml_diff>

<commit_message>
working preALU, and got the truth tables
</commit_message>
<xml_diff>
--- a/projects/02/ALU Debugger.xlsx
+++ b/projects/02/ALU Debugger.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Debugger" sheetId="1" r:id="rId1"/>
     <sheet name="No Stat Tests" sheetId="2" r:id="rId2"/>
+    <sheet name="Truth Tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="testNo">'ALU Debugger'!$B$3</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
   <si>
     <t>x input</t>
   </si>
@@ -157,12 +158,48 @@
   <si>
     <t>Carry</t>
   </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Pre ALU - Truth Table</t>
+  </si>
+  <si>
+    <t>Mid ALU - Truth Table</t>
+  </si>
+  <si>
+    <t>carry</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +246,17 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="monti"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -236,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -324,11 +372,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -429,6 +526,37 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AI16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10385,4 +10513,1152 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" style="45" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="49"/>
+    <col min="6" max="16384" width="9.140625" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="44">
+        <v>0</v>
+      </c>
+      <c r="C5" s="44">
+        <v>0</v>
+      </c>
+      <c r="D5" s="48">
+        <v>0</v>
+      </c>
+      <c r="E5" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="44">
+        <v>0</v>
+      </c>
+      <c r="D6" s="48">
+        <v>1</v>
+      </c>
+      <c r="E6" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="44">
+        <v>0</v>
+      </c>
+      <c r="C7" s="44">
+        <v>1</v>
+      </c>
+      <c r="D7" s="48">
+        <v>0</v>
+      </c>
+      <c r="E7" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="44">
+        <v>0</v>
+      </c>
+      <c r="C8" s="44">
+        <v>1</v>
+      </c>
+      <c r="D8" s="48">
+        <v>1</v>
+      </c>
+      <c r="E8" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="44">
+        <v>0</v>
+      </c>
+      <c r="D9" s="48">
+        <v>0</v>
+      </c>
+      <c r="E9" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="44">
+        <v>1</v>
+      </c>
+      <c r="C10" s="44">
+        <v>0</v>
+      </c>
+      <c r="D10" s="48">
+        <v>1</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="44">
+        <v>1</v>
+      </c>
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
+      <c r="D11" s="48">
+        <v>0</v>
+      </c>
+      <c r="E11" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="44">
+        <v>1</v>
+      </c>
+      <c r="C12" s="44">
+        <v>1</v>
+      </c>
+      <c r="D12" s="48">
+        <v>1</v>
+      </c>
+      <c r="E12" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" s="50">
+        <v>0</v>
+      </c>
+      <c r="C17" s="50">
+        <v>0</v>
+      </c>
+      <c r="D17" s="50">
+        <v>0</v>
+      </c>
+      <c r="E17" s="50">
+        <v>0</v>
+      </c>
+      <c r="F17" s="51">
+        <v>0</v>
+      </c>
+      <c r="G17" s="50">
+        <v>0</v>
+      </c>
+      <c r="H17" s="50">
+        <v>0</v>
+      </c>
+      <c r="J17" s="45">
+        <v>0</v>
+      </c>
+      <c r="K17" s="53" t="str">
+        <f>DEC2BIN(J17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" s="52">
+        <v>0</v>
+      </c>
+      <c r="C18" s="52">
+        <v>0</v>
+      </c>
+      <c r="D18" s="52">
+        <v>0</v>
+      </c>
+      <c r="E18" s="52">
+        <v>0</v>
+      </c>
+      <c r="F18" s="48">
+        <v>1</v>
+      </c>
+      <c r="G18" s="44">
+        <v>0</v>
+      </c>
+      <c r="H18" s="44">
+        <v>0</v>
+      </c>
+      <c r="J18" s="45">
+        <v>1</v>
+      </c>
+      <c r="K18" s="53" t="str">
+        <f>DEC2BIN(J18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="52">
+        <v>0</v>
+      </c>
+      <c r="C19" s="52">
+        <v>0</v>
+      </c>
+      <c r="D19" s="52">
+        <v>0</v>
+      </c>
+      <c r="E19" s="52">
+        <v>1</v>
+      </c>
+      <c r="F19" s="48">
+        <v>0</v>
+      </c>
+      <c r="G19" s="44">
+        <v>0</v>
+      </c>
+      <c r="H19" s="44">
+        <v>0</v>
+      </c>
+      <c r="J19" s="45">
+        <v>2</v>
+      </c>
+      <c r="K19" s="53" t="str">
+        <f t="shared" ref="K18:K48" si="0">DEC2BIN(J19)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="52">
+        <v>0</v>
+      </c>
+      <c r="C20" s="52">
+        <v>0</v>
+      </c>
+      <c r="D20" s="52">
+        <v>0</v>
+      </c>
+      <c r="E20" s="52">
+        <v>1</v>
+      </c>
+      <c r="F20" s="48">
+        <v>1</v>
+      </c>
+      <c r="G20" s="44">
+        <v>0</v>
+      </c>
+      <c r="H20" s="44">
+        <v>0</v>
+      </c>
+      <c r="J20" s="45">
+        <v>3</v>
+      </c>
+      <c r="K20" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="52">
+        <v>0</v>
+      </c>
+      <c r="C21" s="52">
+        <v>0</v>
+      </c>
+      <c r="D21" s="52">
+        <v>1</v>
+      </c>
+      <c r="E21" s="52">
+        <v>0</v>
+      </c>
+      <c r="F21" s="48">
+        <v>0</v>
+      </c>
+      <c r="G21" s="44">
+        <v>0</v>
+      </c>
+      <c r="H21" s="44">
+        <v>0</v>
+      </c>
+      <c r="J21" s="45">
+        <v>4</v>
+      </c>
+      <c r="K21" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="52">
+        <v>0</v>
+      </c>
+      <c r="C22" s="52">
+        <v>0</v>
+      </c>
+      <c r="D22" s="52">
+        <v>1</v>
+      </c>
+      <c r="E22" s="52">
+        <v>0</v>
+      </c>
+      <c r="F22" s="48">
+        <v>1</v>
+      </c>
+      <c r="G22" s="44">
+        <v>0</v>
+      </c>
+      <c r="H22" s="44">
+        <v>0</v>
+      </c>
+      <c r="J22" s="45">
+        <v>5</v>
+      </c>
+      <c r="K22" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="52">
+        <v>0</v>
+      </c>
+      <c r="C23" s="52">
+        <v>0</v>
+      </c>
+      <c r="D23" s="52">
+        <v>1</v>
+      </c>
+      <c r="E23" s="52">
+        <v>1</v>
+      </c>
+      <c r="F23" s="48">
+        <v>0</v>
+      </c>
+      <c r="G23" s="44">
+        <v>0</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0</v>
+      </c>
+      <c r="J23" s="45">
+        <v>6</v>
+      </c>
+      <c r="K23" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="52">
+        <v>0</v>
+      </c>
+      <c r="C24" s="52">
+        <v>0</v>
+      </c>
+      <c r="D24" s="52">
+        <v>1</v>
+      </c>
+      <c r="E24" s="52">
+        <v>1</v>
+      </c>
+      <c r="F24" s="48">
+        <v>1</v>
+      </c>
+      <c r="G24" s="44">
+        <v>0</v>
+      </c>
+      <c r="H24" s="44">
+        <v>0</v>
+      </c>
+      <c r="J24" s="45">
+        <v>7</v>
+      </c>
+      <c r="K24" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="52">
+        <v>0</v>
+      </c>
+      <c r="C25" s="52">
+        <v>1</v>
+      </c>
+      <c r="D25" s="52">
+        <v>0</v>
+      </c>
+      <c r="E25" s="52">
+        <v>0</v>
+      </c>
+      <c r="F25" s="48">
+        <v>0</v>
+      </c>
+      <c r="G25" s="44">
+        <v>0</v>
+      </c>
+      <c r="H25" s="44">
+        <v>0</v>
+      </c>
+      <c r="J25" s="45">
+        <v>8</v>
+      </c>
+      <c r="K25" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="52">
+        <v>0</v>
+      </c>
+      <c r="C26" s="52">
+        <v>1</v>
+      </c>
+      <c r="D26" s="52">
+        <v>0</v>
+      </c>
+      <c r="E26" s="52">
+        <v>0</v>
+      </c>
+      <c r="F26" s="48">
+        <v>1</v>
+      </c>
+      <c r="G26" s="44">
+        <v>0</v>
+      </c>
+      <c r="H26" s="44">
+        <v>0</v>
+      </c>
+      <c r="J26" s="45">
+        <v>9</v>
+      </c>
+      <c r="K26" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="52">
+        <v>0</v>
+      </c>
+      <c r="C27" s="52">
+        <v>1</v>
+      </c>
+      <c r="D27" s="52">
+        <v>0</v>
+      </c>
+      <c r="E27" s="52">
+        <v>1</v>
+      </c>
+      <c r="F27" s="48">
+        <v>0</v>
+      </c>
+      <c r="G27" s="44">
+        <v>0</v>
+      </c>
+      <c r="H27" s="44">
+        <v>0</v>
+      </c>
+      <c r="J27" s="45">
+        <v>10</v>
+      </c>
+      <c r="K27" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="52">
+        <v>0</v>
+      </c>
+      <c r="C28" s="52">
+        <v>1</v>
+      </c>
+      <c r="D28" s="52">
+        <v>0</v>
+      </c>
+      <c r="E28" s="52">
+        <v>1</v>
+      </c>
+      <c r="F28" s="48">
+        <v>1</v>
+      </c>
+      <c r="G28" s="44">
+        <v>0</v>
+      </c>
+      <c r="H28" s="44">
+        <v>0</v>
+      </c>
+      <c r="J28" s="45">
+        <v>11</v>
+      </c>
+      <c r="K28" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="52">
+        <v>0</v>
+      </c>
+      <c r="C29" s="52">
+        <v>1</v>
+      </c>
+      <c r="D29" s="52">
+        <v>1</v>
+      </c>
+      <c r="E29" s="52">
+        <v>0</v>
+      </c>
+      <c r="F29" s="48">
+        <v>0</v>
+      </c>
+      <c r="G29" s="44">
+        <v>0</v>
+      </c>
+      <c r="H29" s="44">
+        <v>0</v>
+      </c>
+      <c r="J29" s="45">
+        <v>12</v>
+      </c>
+      <c r="K29" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="52">
+        <v>0</v>
+      </c>
+      <c r="C30" s="52">
+        <v>1</v>
+      </c>
+      <c r="D30" s="52">
+        <v>1</v>
+      </c>
+      <c r="E30" s="52">
+        <v>0</v>
+      </c>
+      <c r="F30" s="48">
+        <v>1</v>
+      </c>
+      <c r="G30" s="44">
+        <v>0</v>
+      </c>
+      <c r="H30" s="44">
+        <v>0</v>
+      </c>
+      <c r="J30" s="45">
+        <v>13</v>
+      </c>
+      <c r="K30" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="52">
+        <v>0</v>
+      </c>
+      <c r="C31" s="52">
+        <v>1</v>
+      </c>
+      <c r="D31" s="52">
+        <v>1</v>
+      </c>
+      <c r="E31" s="52">
+        <v>1</v>
+      </c>
+      <c r="F31" s="48">
+        <v>0</v>
+      </c>
+      <c r="G31" s="44">
+        <v>0</v>
+      </c>
+      <c r="H31" s="44">
+        <v>0</v>
+      </c>
+      <c r="J31" s="45">
+        <v>14</v>
+      </c>
+      <c r="K31" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="52">
+        <v>0</v>
+      </c>
+      <c r="C32" s="52">
+        <v>1</v>
+      </c>
+      <c r="D32" s="52">
+        <v>1</v>
+      </c>
+      <c r="E32" s="52">
+        <v>1</v>
+      </c>
+      <c r="F32" s="48">
+        <v>1</v>
+      </c>
+      <c r="G32" s="44">
+        <v>0</v>
+      </c>
+      <c r="H32" s="44">
+        <v>0</v>
+      </c>
+      <c r="J32" s="45">
+        <v>15</v>
+      </c>
+      <c r="K32" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="52">
+        <v>1</v>
+      </c>
+      <c r="C33" s="52">
+        <v>0</v>
+      </c>
+      <c r="D33" s="52">
+        <v>0</v>
+      </c>
+      <c r="E33" s="52">
+        <v>0</v>
+      </c>
+      <c r="F33" s="48">
+        <v>0</v>
+      </c>
+      <c r="G33" s="44">
+        <v>0</v>
+      </c>
+      <c r="H33" s="44">
+        <v>0</v>
+      </c>
+      <c r="J33" s="45">
+        <v>16</v>
+      </c>
+      <c r="K33" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="52">
+        <v>1</v>
+      </c>
+      <c r="C34" s="52">
+        <v>0</v>
+      </c>
+      <c r="D34" s="52">
+        <v>0</v>
+      </c>
+      <c r="E34" s="52">
+        <v>0</v>
+      </c>
+      <c r="F34" s="48">
+        <v>1</v>
+      </c>
+      <c r="G34" s="44">
+        <v>0</v>
+      </c>
+      <c r="H34" s="44">
+        <v>0</v>
+      </c>
+      <c r="J34" s="45">
+        <v>17</v>
+      </c>
+      <c r="K34" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="52">
+        <v>1</v>
+      </c>
+      <c r="C35" s="52">
+        <v>0</v>
+      </c>
+      <c r="D35" s="52">
+        <v>0</v>
+      </c>
+      <c r="E35" s="52">
+        <v>1</v>
+      </c>
+      <c r="F35" s="48">
+        <v>0</v>
+      </c>
+      <c r="G35" s="44">
+        <v>0</v>
+      </c>
+      <c r="H35" s="44">
+        <v>0</v>
+      </c>
+      <c r="J35" s="45">
+        <v>18</v>
+      </c>
+      <c r="K35" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10010</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="52">
+        <v>1</v>
+      </c>
+      <c r="C36" s="52">
+        <v>0</v>
+      </c>
+      <c r="D36" s="52">
+        <v>0</v>
+      </c>
+      <c r="E36" s="52">
+        <v>1</v>
+      </c>
+      <c r="F36" s="48">
+        <v>1</v>
+      </c>
+      <c r="G36" s="44">
+        <v>0</v>
+      </c>
+      <c r="H36" s="44">
+        <v>0</v>
+      </c>
+      <c r="J36" s="45">
+        <v>19</v>
+      </c>
+      <c r="K36" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10011</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="52">
+        <v>1</v>
+      </c>
+      <c r="C37" s="52">
+        <v>0</v>
+      </c>
+      <c r="D37" s="52">
+        <v>1</v>
+      </c>
+      <c r="E37" s="52">
+        <v>0</v>
+      </c>
+      <c r="F37" s="48">
+        <v>0</v>
+      </c>
+      <c r="G37" s="44">
+        <v>0</v>
+      </c>
+      <c r="H37" s="44">
+        <v>0</v>
+      </c>
+      <c r="J37" s="45">
+        <v>20</v>
+      </c>
+      <c r="K37" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="52">
+        <v>1</v>
+      </c>
+      <c r="C38" s="52">
+        <v>0</v>
+      </c>
+      <c r="D38" s="52">
+        <v>1</v>
+      </c>
+      <c r="E38" s="52">
+        <v>0</v>
+      </c>
+      <c r="F38" s="48">
+        <v>1</v>
+      </c>
+      <c r="G38" s="44">
+        <v>0</v>
+      </c>
+      <c r="H38" s="44">
+        <v>0</v>
+      </c>
+      <c r="J38" s="45">
+        <v>21</v>
+      </c>
+      <c r="K38" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10101</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="52">
+        <v>1</v>
+      </c>
+      <c r="C39" s="52">
+        <v>0</v>
+      </c>
+      <c r="D39" s="52">
+        <v>1</v>
+      </c>
+      <c r="E39" s="52">
+        <v>1</v>
+      </c>
+      <c r="F39" s="48">
+        <v>0</v>
+      </c>
+      <c r="G39" s="44">
+        <v>0</v>
+      </c>
+      <c r="H39" s="44">
+        <v>0</v>
+      </c>
+      <c r="J39" s="45">
+        <v>22</v>
+      </c>
+      <c r="K39" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10110</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="52">
+        <v>1</v>
+      </c>
+      <c r="C40" s="52">
+        <v>0</v>
+      </c>
+      <c r="D40" s="52">
+        <v>1</v>
+      </c>
+      <c r="E40" s="52">
+        <v>1</v>
+      </c>
+      <c r="F40" s="48">
+        <v>1</v>
+      </c>
+      <c r="G40" s="44">
+        <v>0</v>
+      </c>
+      <c r="H40" s="44">
+        <v>0</v>
+      </c>
+      <c r="J40" s="45">
+        <v>23</v>
+      </c>
+      <c r="K40" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10111</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="52">
+        <v>1</v>
+      </c>
+      <c r="C41" s="52">
+        <v>1</v>
+      </c>
+      <c r="D41" s="52">
+        <v>0</v>
+      </c>
+      <c r="E41" s="52">
+        <v>0</v>
+      </c>
+      <c r="F41" s="48">
+        <v>0</v>
+      </c>
+      <c r="G41" s="44">
+        <v>0</v>
+      </c>
+      <c r="H41" s="44">
+        <v>0</v>
+      </c>
+      <c r="J41" s="45">
+        <v>24</v>
+      </c>
+      <c r="K41" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="52">
+        <v>1</v>
+      </c>
+      <c r="C42" s="52">
+        <v>1</v>
+      </c>
+      <c r="D42" s="52">
+        <v>0</v>
+      </c>
+      <c r="E42" s="52">
+        <v>0</v>
+      </c>
+      <c r="F42" s="48">
+        <v>1</v>
+      </c>
+      <c r="G42" s="44">
+        <v>0</v>
+      </c>
+      <c r="H42" s="44">
+        <v>0</v>
+      </c>
+      <c r="J42" s="45">
+        <v>25</v>
+      </c>
+      <c r="K42" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="52">
+        <v>1</v>
+      </c>
+      <c r="C43" s="52">
+        <v>1</v>
+      </c>
+      <c r="D43" s="52">
+        <v>0</v>
+      </c>
+      <c r="E43" s="52">
+        <v>1</v>
+      </c>
+      <c r="F43" s="48">
+        <v>0</v>
+      </c>
+      <c r="G43" s="44">
+        <v>0</v>
+      </c>
+      <c r="H43" s="44">
+        <v>0</v>
+      </c>
+      <c r="J43" s="45">
+        <v>26</v>
+      </c>
+      <c r="K43" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11010</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="52">
+        <v>1</v>
+      </c>
+      <c r="C44" s="52">
+        <v>1</v>
+      </c>
+      <c r="D44" s="52">
+        <v>0</v>
+      </c>
+      <c r="E44" s="52">
+        <v>1</v>
+      </c>
+      <c r="F44" s="48">
+        <v>1</v>
+      </c>
+      <c r="G44" s="44">
+        <v>0</v>
+      </c>
+      <c r="H44" s="44">
+        <v>0</v>
+      </c>
+      <c r="J44" s="45">
+        <v>27</v>
+      </c>
+      <c r="K44" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11011</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="52">
+        <v>1</v>
+      </c>
+      <c r="C45" s="52">
+        <v>1</v>
+      </c>
+      <c r="D45" s="52">
+        <v>1</v>
+      </c>
+      <c r="E45" s="52">
+        <v>0</v>
+      </c>
+      <c r="F45" s="48">
+        <v>0</v>
+      </c>
+      <c r="G45" s="44">
+        <v>0</v>
+      </c>
+      <c r="H45" s="44">
+        <v>0</v>
+      </c>
+      <c r="J45" s="45">
+        <v>28</v>
+      </c>
+      <c r="K45" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="52">
+        <v>1</v>
+      </c>
+      <c r="C46" s="52">
+        <v>1</v>
+      </c>
+      <c r="D46" s="52">
+        <v>1</v>
+      </c>
+      <c r="E46" s="52">
+        <v>0</v>
+      </c>
+      <c r="F46" s="48">
+        <v>1</v>
+      </c>
+      <c r="G46" s="44">
+        <v>0</v>
+      </c>
+      <c r="H46" s="44">
+        <v>0</v>
+      </c>
+      <c r="J46" s="45">
+        <v>29</v>
+      </c>
+      <c r="K46" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11101</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="52">
+        <v>1</v>
+      </c>
+      <c r="C47" s="52">
+        <v>1</v>
+      </c>
+      <c r="D47" s="52">
+        <v>1</v>
+      </c>
+      <c r="E47" s="52">
+        <v>1</v>
+      </c>
+      <c r="F47" s="48">
+        <v>0</v>
+      </c>
+      <c r="G47" s="44">
+        <v>0</v>
+      </c>
+      <c r="H47" s="44">
+        <v>0</v>
+      </c>
+      <c r="J47" s="45">
+        <v>30</v>
+      </c>
+      <c r="K47" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11110</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="52">
+        <v>1</v>
+      </c>
+      <c r="C48" s="52">
+        <v>1</v>
+      </c>
+      <c r="D48" s="52">
+        <v>1</v>
+      </c>
+      <c r="E48" s="52">
+        <v>1</v>
+      </c>
+      <c r="F48" s="48">
+        <v>1</v>
+      </c>
+      <c r="G48" s="44">
+        <v>0</v>
+      </c>
+      <c r="H48" s="44">
+        <v>0</v>
+      </c>
+      <c r="J48" s="45">
+        <v>31</v>
+      </c>
+      <c r="K48" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>